<commit_message>
Updated BOM for TMC V1.2.2 hall and STM V1.2.4
</commit_message>
<xml_diff>
--- a/OpenFFBoard-main/V1.2.4 F407/Assembly/BOM_FFBoard.xlsx
+++ b/OpenFFBoard-main/V1.2.4 F407/Assembly/BOM_FFBoard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\git\OpenFFBoard-hardware\OpenFFBoard-main\V1.2.4 F407\Assembly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64AF080-0E33-4C4D-8454-0C61A1F87E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE196638-CE7F-4187-AC52-3ED74FEDE785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5415" yWindow="5415" windowWidth="28800" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -329,7 +329,7 @@
     <t>C2827654</t>
   </si>
   <si>
-    <t>C2293</t>
+    <t>C189307</t>
   </si>
 </sst>
 </file>
@@ -752,7 +752,7 @@
   <dimension ref="A1:AMK25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>

</xml_diff>